<commit_message>
Hyp + état 5 + massflow
</commit_message>
<xml_diff>
--- a/Param/Projet_contraintes.xlsx
+++ b/Param/Projet_contraintes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julem\Dropbox\EPL\Master_1\Q1\LELME2150 Thermal Cycles\2024\Projet\Param\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisevaessen/Documents/Thermal_Project/Param/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946C17EF-FF05-408A-AA44-3EEEF5274CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA477D26-DEEB-FE49-9DF0-3476F6E56640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="615" windowWidth="21600" windowHeight="11385" xr2:uid="{CB6374FC-8A30-4020-B8B5-DB38D12B49A4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CB6374FC-8A30-4020-B8B5-DB38D12B49A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>T_max</t>
   </si>
@@ -143,13 +139,22 @@
     <t>T_pinch_evap_I</t>
   </si>
   <si>
-    <t>diofférence T entre sortie de l'evaporateur I et etat 1</t>
-  </si>
-  <si>
     <t>T_hot_fluid_in_II</t>
   </si>
   <si>
     <t>p_hot_fluid</t>
+  </si>
+  <si>
+    <t>T_cd_subcool</t>
+  </si>
+  <si>
+    <t>différence T entre sortie de l'evaporateur I et etat 1</t>
+  </si>
+  <si>
+    <t>Limite technologique de la turbine</t>
+  </si>
+  <si>
+    <t>p_3</t>
   </si>
 </sst>
 </file>
@@ -586,17 +591,17 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -619,7 +624,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -633,7 +638,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -653,7 +658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -667,7 +672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -681,7 +686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -692,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -703,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -717,7 +722,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -731,7 +736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -745,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -760,7 +765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -774,7 +779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -788,13 +793,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14">
-        <f>273.15+10</f>
-        <v>283.14999999999998</v>
+        <f>273.15+8</f>
+        <v>281.14999999999998</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -803,13 +808,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15">
-        <f>273.15+20</f>
-        <v>293.14999999999998</v>
+        <f>273.15+28</f>
+        <v>301.14999999999998</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -818,9 +823,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <f>140+273.15</f>
@@ -833,13 +838,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
-        <f>140+273.15</f>
-        <v>413.15</v>
+        <f>838.15</f>
+        <v>838.15</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -847,8 +852,11 @@
       <c r="D17" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -859,10 +867,10 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -876,73 +884,104 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>1000000</v>
       </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22">
+        <f>310*10^5</f>
+        <v>31000000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D23" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D24" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D25" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D26" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D27" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D28" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D29" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D30" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D31" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D32" s="2" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Correction eta (pas encore bon)
</commit_message>
<xml_diff>
--- a/Param/Projet_contraintes.xlsx
+++ b/Param/Projet_contraintes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisevaessen/Documents/Thermal_Project/Param/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julem\Dropbox\EPL\Master_1\Q1\LELME2150 Thermal Cycles\2024\Projet\Param\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94AFA90-C675-DE45-8C9E-48C4229D1F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C885A0EC-463C-4541-A594-35F99C58F663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -275,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -292,6 +296,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -314,8 +324,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:F60" totalsRowShown="0">
   <autoFilter ref="A1:F60" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
-    <sortCondition ref="A1:A28"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F60">
+    <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
@@ -619,21 +629,21 @@
   </sheetPr>
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -670,7 +680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -690,26 +700,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.85</v>
+        <v>56</v>
+      </c>
+      <c r="B4" s="2">
+        <f>0.9</f>
+        <v>0.9</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3">
         <v>0.85</v>
@@ -721,48 +729,48 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>23</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -771,29 +779,29 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B11" s="5">
         <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="2">
-        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
@@ -801,455 +809,460 @@
       <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
+    </row>
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="3">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="5">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="2">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="3">
+        <f>1*100000</f>
+        <v>100000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="2">
+        <f>2*1000000</f>
+        <v>2000000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2">
+        <f>2*10^6</f>
+        <v>2000000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="5">
+        <f>0.5*100000</f>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="5">
+        <f>1*100000</f>
+        <v>100000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B22" s="5">
         <f>101325</f>
         <v>101325</v>
       </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="2">
-        <f>2*10^6</f>
-        <v>2000000</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="5">
-        <f>1*100000</f>
-        <v>100000</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="2">
+        <f>1*1000000</f>
         <v>1000000</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="4">
+        <v>31000000</v>
+      </c>
+      <c r="C24" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="4">
-        <v>31000000</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B25" s="8">
         <f>100000</f>
         <v>100000</v>
       </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B26" s="9">
         <f>273.15 + 25</f>
         <v>298.14999999999998</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C26" t="s">
         <v>31</v>
       </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B27" s="9">
         <f>273.15 + 15</f>
         <v>288.14999999999998</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C27" t="s">
         <v>31</v>
       </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B28" s="9">
         <f>273.15 + 140</f>
         <v>413.15</v>
       </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B29" s="9">
         <f>273.15 + 90</f>
         <v>363.15</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B30" s="9">
         <f>273.15 + 40</f>
         <v>313.14999999999998</v>
       </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B31" s="8">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C31" t="s">
         <v>31</v>
       </c>
-      <c r="D23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B32" s="9">
         <f>838.15</f>
         <v>838.15</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C32" t="s">
         <v>31</v>
       </c>
-      <c r="D24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B34" s="6">
         <v>1</v>
       </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B35" s="6">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B36" s="7">
         <f>273.16</f>
         <v>273.16000000000003</v>
       </c>
-      <c r="D28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="6">
-        <f>1*1000000</f>
-        <v>1000000</v>
-      </c>
-      <c r="D29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="7">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="6">
-        <f>0.9</f>
-        <v>0.9</v>
-      </c>
-      <c r="D31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B37" s="7">
         <v>40</v>
       </c>
-      <c r="D32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="6">
-        <v>20</v>
-      </c>
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="7">
-        <f>1*100000</f>
-        <v>100000</v>
-      </c>
-      <c r="D34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="6">
-        <f>2*100000</f>
-        <v>200000</v>
-      </c>
-      <c r="D35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="1">
-        <f>0.5*100000</f>
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="1">
-        <v>10</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="D42" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="D43" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="D44" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="D45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
       <c r="D46" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="D47" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="D48" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="D49" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="D50" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="D51" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
       <c r="D52" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="D53" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
       <c r="D54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="D55" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="D56" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="D57" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
       <c r="D58" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="D59" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
       <c r="D60" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Jules Propal en plus
</commit_message>
<xml_diff>
--- a/Param/Projet_contraintes.xlsx
+++ b/Param/Projet_contraintes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisevaessen/Documents/Thermal_Project/Param/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julem\Dropbox\EPL\Master_1\Q1\LELME2150 Thermal Cycles\2024\Projet\Param\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95D21E0-729E-044C-B493-BB86EA06D916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1482E0-7B75-48E7-9BF0-7DD77DA6F5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8310" yWindow="1845" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -233,6 +237,9 @@
   </si>
   <si>
     <t>T_pinch = 10</t>
+  </si>
+  <si>
+    <t>NOT USED</t>
   </si>
 </sst>
 </file>
@@ -290,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -307,6 +314,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -329,8 +342,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:F60" totalsRowShown="0">
   <autoFilter ref="A1:F60" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
-    <sortCondition ref="A1:A28"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F60">
+    <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
@@ -634,21 +647,21 @@
   </sheetPr>
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -671,7 +684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -685,7 +698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -705,26 +718,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.85</v>
+        <v>55</v>
+      </c>
+      <c r="B4" s="2">
+        <f>8*10^(-1)</f>
+        <v>0.8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3">
         <v>0.85</v>
@@ -736,48 +747,48 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>23</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -786,29 +797,29 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B11" s="5">
         <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="2">
-        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
@@ -816,473 +827,498 @@
       <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
+    </row>
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="3">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="5">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="3">
+        <f>1*500000</f>
+        <v>500000</v>
+      </c>
+      <c r="C16">
+        <f>Tableau1[[#This Row],[Value]]/100000</f>
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="2">
+        <f>2*1000000</f>
+        <v>2000000</v>
+      </c>
+      <c r="C17">
+        <f>Tableau1[[#This Row],[Value]]/100000</f>
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2">
+        <f>2*10^6</f>
+        <v>2000000</v>
+      </c>
+      <c r="C18">
+        <f>Tableau1[[#This Row],[Value]]/100000</f>
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="5">
+        <f>0.5*100000</f>
+        <v>50000</v>
+      </c>
+      <c r="C19">
+        <f>Tableau1[[#This Row],[Value]]/100000</f>
+        <v>0.5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="5">
+        <f>1*100000</f>
+        <v>100000</v>
+      </c>
+      <c r="C20">
+        <f>Tableau1[[#This Row],[Value]]/100000</f>
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B22" s="5">
         <f>101325</f>
         <v>101325</v>
       </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="2">
-        <f>2*10^6</f>
-        <v>2000000</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="5">
-        <f>1*100000</f>
-        <v>100000</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="2">
+        <f>10*10^5</f>
         <v>1000000</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="4">
+        <v>31000000</v>
+      </c>
+      <c r="C24" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="4">
-        <v>31000000</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B25" s="8">
         <f>100000</f>
         <v>100000</v>
       </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
         <v>16</v>
       </c>
-      <c r="H17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    </row>
+    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B26" s="9">
         <f>273.15 + 25</f>
         <v>298.14999999999998</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C26" t="s">
         <v>31</v>
       </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B27" s="9">
         <f>273.15 + 15</f>
         <v>288.14999999999998</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C27" t="s">
         <v>31</v>
       </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B28" s="9">
         <f>273.15 + 140</f>
         <v>413.15</v>
       </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B29" s="9">
         <f>273.15 + 90</f>
         <v>363.15</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B30" s="9">
         <f>273.15 + 40</f>
         <v>313.14999999999998</v>
       </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B31" s="8">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C31" t="s">
         <v>31</v>
       </c>
-      <c r="D23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B32" s="9">
         <f>838.15</f>
         <v>838.15</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C32" t="s">
         <v>31</v>
       </c>
-      <c r="D24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B33" s="1">
         <v>10</v>
       </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B34" s="6">
         <v>10</v>
       </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B35" s="6">
         <f>10</f>
         <v>10</v>
       </c>
-      <c r="D27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B36" s="7">
         <f>273.16</f>
         <v>273.16000000000003</v>
       </c>
-      <c r="D28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="6">
-        <f>10*10^5</f>
-        <v>1000000</v>
-      </c>
-      <c r="D29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="7">
-        <v>100</v>
-      </c>
-      <c r="D30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="6">
-        <f>8*10^(-1)</f>
-        <v>0.8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B37" s="7">
         <v>30</v>
       </c>
-      <c r="D32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="6">
-        <v>20</v>
-      </c>
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="7">
-        <f>1*100000</f>
-        <v>100000</v>
-      </c>
-      <c r="D34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="6">
-        <f>2*100000</f>
-        <v>200000</v>
-      </c>
-      <c r="D35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="1">
-        <f>0.5*100000</f>
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="1">
-        <v>10</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
       <c r="D42" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="D43" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="D44" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="D45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" s="7"/>
       <c r="D46" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
       <c r="D47" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
       <c r="D48" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="6"/>
       <c r="D49" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
       <c r="D50" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
       <c r="D51" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
       <c r="D52" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="D53" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
       <c r="D54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="D55" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
       <c r="D56" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="D57" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
       <c r="D58" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="6"/>
       <c r="D59" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
       <c r="D60" t="s">
         <v>9</v>

</xml_diff>